<commit_message>
Camera controls added but models buggy
</commit_message>
<xml_diff>
--- a/Level Renderer Project/Project Rubric.xlsx
+++ b/Level Renderer Project/Project Rubric.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e87c385a0523d84e/Documents/Full Sail/3D Content Creation/3dcc-course-materials-CodeWithJazmine/Level Renderer Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="96" documentId="13_ncr:1_{3BA54DA0-33D1-42D2-A2A2-AD35B96A3236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6C7648A-CBCB-418E-93B6-5265E59C15C6}"/>
+  <xr:revisionPtr revIDLastSave="108" documentId="13_ncr:1_{3BA54DA0-33D1-42D2-A2A2-AD35B96A3236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06F44810-1B2B-40EB-9844-29E73CEC4528}"/>
   <bookViews>
-    <workbookView xWindow="4035" yWindow="1845" windowWidth="21930" windowHeight="17040" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
+    <workbookView xWindow="9555" yWindow="1230" windowWidth="20745" windowHeight="18090" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1539,7 +1539,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
   <si>
     <t>1. One or More Blender Game Levels to export from (.blend)</t>
   </si>
@@ -1701,6 +1701,15 @@
   </si>
   <si>
     <t>Fully complete 7 or more Key Features</t>
+  </si>
+  <si>
+    <t>Note: specular lights must react to camera movements</t>
+  </si>
+  <si>
+    <t>I want to do this</t>
+  </si>
+  <si>
+    <t>Doing this</t>
   </si>
 </sst>
 </file>
@@ -2058,6 +2067,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
@@ -2355,10 +2368,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A40538-A3BB-461B-BC01-A04BD38DD6FA}">
-  <dimension ref="A1:C55"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2367,7 +2380,7 @@
     <col min="2" max="3" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -2378,7 +2391,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
@@ -2389,7 +2402,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>1</v>
       </c>
@@ -2400,7 +2413,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>29</v>
       </c>
@@ -2411,7 +2424,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>30</v>
       </c>
@@ -2422,7 +2435,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -2433,7 +2446,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -2444,7 +2457,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>39</v>
       </c>
@@ -2455,7 +2468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>33</v>
       </c>
@@ -2466,7 +2479,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>34</v>
       </c>
@@ -2477,7 +2490,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>52</v>
       </c>
@@ -2485,10 +2498,13 @@
         <v>0.05</v>
       </c>
       <c r="C11" s="3">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="D11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>4</v>
       </c>
@@ -2498,10 +2514,10 @@
       </c>
       <c r="C12" s="6">
         <f>SUM(C2:C11)</f>
-        <v>0.47000000000000003</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+        <v>0.42000000000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>45</v>
       </c>
@@ -2512,7 +2528,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
         <v>19</v>
       </c>
@@ -2523,7 +2539,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
         <v>7</v>
       </c>
@@ -2534,7 +2550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
         <v>51</v>
       </c>
@@ -2545,7 +2561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="23" t="s">
         <v>8</v>
       </c>
@@ -2556,7 +2572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>46</v>
       </c>
@@ -2566,8 +2582,11 @@
       <c r="C18" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>6</v>
       </c>
@@ -2577,8 +2596,11 @@
       <c r="C19" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>49</v>
       </c>
@@ -2588,8 +2610,11 @@
       <c r="C20" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
         <v>40</v>
       </c>
@@ -2600,7 +2625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>44</v>
       </c>
@@ -2611,7 +2636,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
         <v>10</v>
       </c>
@@ -2622,7 +2647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>27</v>
       </c>
@@ -2633,7 +2658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
         <v>9</v>
       </c>
@@ -2644,7 +2669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="22" t="s">
         <v>50</v>
       </c>
@@ -2655,7 +2680,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
         <v>37</v>
       </c>
@@ -2666,7 +2691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>18</v>
       </c>
@@ -2677,7 +2702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
         <v>4</v>
       </c>
@@ -2689,7 +2714,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>48</v>
       </c>
@@ -2700,7 +2725,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A31" s="24" t="s">
         <v>41</v>
       </c>
@@ -2711,7 +2736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="24" t="s">
         <v>53</v>
       </c>
@@ -2722,7 +2747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>38</v>
       </c>
@@ -2732,8 +2757,11 @@
       <c r="C33" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>43</v>
       </c>
@@ -2744,7 +2772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>11</v>
       </c>
@@ -2755,7 +2783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>12</v>
       </c>
@@ -2766,7 +2794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>23</v>
       </c>
@@ -2777,7 +2805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>28</v>
       </c>
@@ -2788,7 +2816,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
         <v>14</v>
       </c>
@@ -2799,7 +2827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="17" t="s">
         <v>25</v>
       </c>
@@ -2810,7 +2838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="17" t="s">
         <v>15</v>
       </c>
@@ -2821,7 +2849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="17" t="s">
         <v>31</v>
       </c>
@@ -2832,7 +2860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="17" t="s">
         <v>16</v>
       </c>
@@ -2843,7 +2871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="17" t="s">
         <v>17</v>
       </c>
@@ -2854,7 +2882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="17" t="s">
         <v>24</v>
       </c>
@@ -2865,7 +2893,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="17" t="s">
         <v>26</v>
       </c>
@@ -2876,7 +2904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="17" t="s">
         <v>32</v>
       </c>
@@ -2887,7 +2915,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="11" t="s">
         <v>13</v>
       </c>
@@ -2898,7 +2926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>4</v>
       </c>
@@ -2910,7 +2938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>47</v>
       </c>
@@ -2921,7 +2949,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A51" s="20" t="s">
         <v>36</v>
       </c>
@@ -2931,8 +2959,11 @@
       <c r="C51" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D51" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="20" t="s">
         <v>42</v>
       </c>
@@ -2942,8 +2973,11 @@
       <c r="C52" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D52" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="21" t="s">
         <v>35</v>
       </c>
@@ -2953,8 +2987,11 @@
       <c r="C53" s="7">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D53" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="12" t="s">
         <v>4</v>
       </c>
@@ -2967,7 +3004,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="14" t="s">
         <v>20</v>
       </c>
@@ -2977,7 +3014,7 @@
       </c>
       <c r="C55" s="16">
         <f>MIN(SUM(C54,C49,C29,C12),100%)</f>
-        <v>0.47000000000000003</v>
+        <v>0.42000000000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
All materials now load in correctly
</commit_message>
<xml_diff>
--- a/Level Renderer Project/Project Rubric.xlsx
+++ b/Level Renderer Project/Project Rubric.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e87c385a0523d84e/Documents/Full Sail/3D Content Creation/3dcc-course-materials-CodeWithJazmine/Level Renderer Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="108" documentId="13_ncr:1_{3BA54DA0-33D1-42D2-A2A2-AD35B96A3236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{06F44810-1B2B-40EB-9844-29E73CEC4528}"/>
+  <xr:revisionPtr revIDLastSave="111" documentId="13_ncr:1_{3BA54DA0-33D1-42D2-A2A2-AD35B96A3236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{225911D9-1E4B-4BE3-94C4-AA736FCE4339}"/>
   <bookViews>
-    <workbookView xWindow="9555" yWindow="1230" windowWidth="20745" windowHeight="18090" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
+    <workbookView xWindow="3795" yWindow="375" windowWidth="25155" windowHeight="18090" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1539,7 +1539,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="58">
   <si>
     <t>1. One or More Blender Game Levels to export from (.blend)</t>
   </si>
@@ -1710,6 +1710,9 @@
   </si>
   <si>
     <t>Doing this</t>
+  </si>
+  <si>
+    <t>Need a README.txt file of controls!</t>
   </si>
 </sst>
 </file>
@@ -2371,7 +2374,7 @@
   <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2465,7 +2468,10 @@
         <v>0.03</v>
       </c>
       <c r="C8" s="3">
-        <v>0</v>
+        <v>0.02</v>
+      </c>
+      <c r="D8" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2514,7 +2520,7 @@
       </c>
       <c r="C12" s="6">
         <f>SUM(C2:C11)</f>
-        <v>0.42000000000000004</v>
+        <v>0.43999999999999995</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -3014,7 +3020,7 @@
       </c>
       <c r="C55" s="16">
         <f>MIN(SUM(C54,C49,C29,C12),100%)</f>
-        <v>0.42000000000000004</v>
+        <v>0.43999999999999995</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moved Camera controls to Camera.h
</commit_message>
<xml_diff>
--- a/Level Renderer Project/Project Rubric.xlsx
+++ b/Level Renderer Project/Project Rubric.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e87c385a0523d84e/Documents/Full Sail/3D Content Creation/3dcc-course-materials-CodeWithJazmine/Level Renderer Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="118" documentId="13_ncr:1_{3BA54DA0-33D1-42D2-A2A2-AD35B96A3236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD13904B-F590-4631-967C-3C79990F0B74}"/>
+  <xr:revisionPtr revIDLastSave="144" documentId="13_ncr:1_{3BA54DA0-33D1-42D2-A2A2-AD35B96A3236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4DFC2E6A-A2D3-408D-BCC0-9F504B498C24}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
+    <workbookView xWindow="15120" yWindow="1530" windowWidth="19110" windowHeight="18090" xr2:uid="{2B9022D0-B5E6-432E-8A19-30BD25892E64}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1539,7 +1539,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="55">
   <si>
     <t>1. One or More Blender Game Levels to export from (.blend)</t>
   </si>
@@ -1704,9 +1704,6 @@
   </si>
   <si>
     <t>I want to do this</t>
-  </si>
-  <si>
-    <t>Doing this</t>
   </si>
 </sst>
 </file>
@@ -2064,6 +2061,10 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
@@ -2363,8 +2364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A40538-A3BB-461B-BC01-A04BD38DD6FA}">
   <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2373,7 +2374,7 @@
     <col min="2" max="3" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>22</v>
       </c>
@@ -2384,7 +2385,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
@@ -2395,7 +2396,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>1</v>
       </c>
@@ -2406,7 +2407,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>29</v>
       </c>
@@ -2417,7 +2418,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
         <v>30</v>
       </c>
@@ -2428,7 +2429,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
@@ -2439,7 +2440,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
@@ -2450,7 +2451,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>39</v>
       </c>
@@ -2461,7 +2462,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>33</v>
       </c>
@@ -2472,7 +2473,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>34</v>
       </c>
@@ -2483,7 +2484,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>52</v>
       </c>
@@ -2494,7 +2495,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>4</v>
       </c>
@@ -2507,7 +2508,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>45</v>
       </c>
@@ -2518,7 +2519,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A14" s="23" t="s">
         <v>19</v>
       </c>
@@ -2526,10 +2527,13 @@
         <v>0.05</v>
       </c>
       <c r="C14" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.05</v>
+      </c>
+      <c r="D14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
         <v>7</v>
       </c>
@@ -2540,7 +2544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
         <v>51</v>
       </c>
@@ -2572,9 +2576,6 @@
       <c r="C18" s="3">
         <v>0</v>
       </c>
-      <c r="D18" t="s">
-        <v>54</v>
-      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
@@ -2586,9 +2587,6 @@
       <c r="C19" s="3">
         <v>0</v>
       </c>
-      <c r="D19" t="s">
-        <v>54</v>
-      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
@@ -2669,6 +2667,9 @@
       <c r="C26" s="3">
         <v>0</v>
       </c>
+      <c r="D26" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="18" t="s">
@@ -2701,7 +2702,7 @@
       </c>
       <c r="C29" s="6">
         <f>MIN(SUM(C14:C28),33%)</f>
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -2963,9 +2964,6 @@
       <c r="C52" s="3">
         <v>0</v>
       </c>
-      <c r="D52" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="53" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="21" t="s">
@@ -3004,7 +3002,7 @@
       </c>
       <c r="C55" s="16">
         <f>MIN(SUM(C54,C49,C29,C12),100%)</f>
-        <v>0.54999999999999993</v>
+        <v>0.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>